<commit_message>
HW sintetizando corretamente com 8 canais
</commit_message>
<xml_diff>
--- a/LVDS Buffers/HSMC_B_Pinout.xlsx
+++ b/LVDS Buffers/HSMC_B_Pinout.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfranca\Dev\GitHub\SimuCam_Development\LVDS Buffers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfranca\Development\GitHub\SimuCam_Development\LVDS Buffers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855" firstSheet="5" activeTab="6" xr2:uid="{5A5778FA-B7D5-4E74-ADCB-8E59276416A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DE4 HSMC B Pinout" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SpaceWire - Axon Conector'!$B$2:$F$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Stratix IV GX Pin Mapping'!$B$2:$H$69</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1744,7 +1744,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1794,10 +1794,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2077,7 +2077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F163"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -2094,13 +2094,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -4849,7 +4849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A2:F252"/>
   <sheetViews>
@@ -6429,7 +6429,7 @@
       <c r="A252" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C162" xr:uid="{6B1E055E-E4AD-4CA9-BECC-E3C88971B1F5}">
+  <autoFilter ref="B2:C162">
     <filterColumn colId="1">
       <filters>
         <filter val="TX13_PD"/>
@@ -6441,11 +6441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="C63" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7790,7 +7790,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>437</v>
@@ -8483,13 +8483,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H82" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="B2:H82"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="B2:G58"/>
   <sheetViews>
@@ -8784,7 +8784,7 @@
     <row r="57" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="58" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="B2:E58" xr:uid="{00000000-0009-0000-0000-000004000000}">
+  <autoFilter ref="B2:E58">
     <filterColumn colId="0">
       <filters>
         <filter val="SpW G"/>
@@ -8800,7 +8800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9172,7 +9172,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F20" xr:uid="{00000000-0009-0000-0000-000005000000}">
+  <autoFilter ref="B2:F20">
     <sortState ref="B3:F22">
       <sortCondition ref="E2:E20"/>
     </sortState>
@@ -9182,7 +9182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A829D7B-85B9-4BEE-B1F5-E8ECF0CB652C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9199,7 +9199,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="4" t="s">
         <v>563</v>
       </c>
@@ -9491,15 +9491,15 @@
       </c>
       <c r="E13" s="2" t="str">
         <f t="array" ref="E13">INDEX('LVDS Board Conectors Pinout'!$D$3:$D$82,MATCH(C13&amp;D13,'LVDS Board Conectors Pinout'!$F$3:$F$82&amp;'LVDS Board Conectors Pinout'!$G$3:$G$82,0))</f>
-        <v>TX4_PD</v>
+        <v>TX4_ND</v>
       </c>
       <c r="F13" s="2">
         <f>INDEX('LVDS Board HSMC Pinout'!$B$3:$B$162,MATCH(E13,'LVDS Board HSMC Pinout'!$C$3:$C$162,0))</f>
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G13" s="2" t="str">
         <f>INDEX('DE4 HSMC B Pinout'!$F$4:$F$163,MATCH(F13,'DE4 HSMC B Pinout'!$B$4:$B$163,0))</f>
-        <v>PIN_N12</v>
+        <v>PIN_M12</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>489</v>
@@ -10962,14 +10962,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H69" xr:uid="{0722B5DE-1338-4642-AC9C-E973AF1E5FCA}"/>
+  <autoFilter ref="B2:H69"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD0A7B4-EF46-480B-A233-C7732B3E6E99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -12263,7 +12263,7 @@
       </c>
       <c r="D111" s="2" t="str">
         <f>INDEX('Stratix IV GX Pin Mapping'!$G$3:$G$69,MATCH(B111,'Stratix IV GX Pin Mapping'!$B$3:$B$69,0))</f>
-        <v>PIN_N12</v>
+        <v>PIN_M12</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
@@ -13506,7 +13506,7 @@
       <c r="B268" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D200" xr:uid="{33336FC8-01FF-4171-9854-FA1EA74E0004}">
+  <autoFilter ref="B2:D200">
     <sortState ref="B3:D200">
       <sortCondition ref="B2:B200"/>
     </sortState>

</xml_diff>

<commit_message>
Testes realizados com as três placas de Buffer LVDS, todos os canais nas três placas funcionando corretamente
</commit_message>
<xml_diff>
--- a/LVDS Buffers/HSMC_B_Pinout.xlsx
+++ b/LVDS Buffers/HSMC_B_Pinout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DE4 HSMC B Pinout" sheetId="1" r:id="rId1"/>
@@ -9183,9 +9183,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9222,7 +9225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>564</v>
       </c>
@@ -9247,7 +9250,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>560</v>
       </c>
@@ -9272,7 +9275,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>561</v>
       </c>
@@ -9505,7 +9508,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>504</v>
       </c>
@@ -9531,7 +9534,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>505</v>
       </c>
@@ -9557,7 +9560,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>506</v>
       </c>
@@ -9583,7 +9586,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>507</v>
       </c>
@@ -9609,7 +9612,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>508</v>
       </c>
@@ -9635,7 +9638,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>509</v>
       </c>
@@ -9661,7 +9664,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>510</v>
       </c>
@@ -9687,7 +9690,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>511</v>
       </c>
@@ -9713,7 +9716,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>512</v>
       </c>
@@ -9739,7 +9742,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>513</v>
       </c>
@@ -9765,7 +9768,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>514</v>
       </c>
@@ -9791,7 +9794,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>515</v>
       </c>
@@ -9817,7 +9820,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>516</v>
       </c>
@@ -9843,7 +9846,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>517</v>
       </c>
@@ -9869,7 +9872,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>518</v>
       </c>
@@ -9895,7 +9898,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>519</v>
       </c>
@@ -9921,7 +9924,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>520</v>
       </c>
@@ -9947,7 +9950,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>521</v>
       </c>
@@ -9973,7 +9976,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>522</v>
       </c>
@@ -9999,7 +10002,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>523</v>
       </c>
@@ -10025,7 +10028,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>524</v>
       </c>
@@ -10051,7 +10054,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>525</v>
       </c>
@@ -10077,7 +10080,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>526</v>
       </c>
@@ -10103,7 +10106,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>527</v>
       </c>
@@ -10129,7 +10132,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>528</v>
       </c>
@@ -10155,7 +10158,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>529</v>
       </c>
@@ -10181,7 +10184,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>530</v>
       </c>
@@ -10207,7 +10210,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>531</v>
       </c>
@@ -10233,7 +10236,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>532</v>
       </c>
@@ -10259,7 +10262,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>533</v>
       </c>
@@ -10285,7 +10288,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>534</v>
       </c>
@@ -10311,7 +10314,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>535</v>
       </c>
@@ -10337,7 +10340,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>536</v>
       </c>
@@ -10363,7 +10366,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>537</v>
       </c>
@@ -10389,7 +10392,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>538</v>
       </c>
@@ -10415,7 +10418,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>539</v>
       </c>
@@ -10441,7 +10444,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>540</v>
       </c>
@@ -10467,7 +10470,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>541</v>
       </c>
@@ -10493,7 +10496,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>542</v>
       </c>
@@ -10519,7 +10522,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>543</v>
       </c>
@@ -10545,7 +10548,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>544</v>
       </c>
@@ -10571,7 +10574,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>545</v>
       </c>
@@ -10597,7 +10600,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>546</v>
       </c>
@@ -10623,7 +10626,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>547</v>
       </c>
@@ -10649,7 +10652,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>548</v>
       </c>
@@ -10675,7 +10678,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>549</v>
       </c>
@@ -10701,7 +10704,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>550</v>
       </c>
@@ -10727,7 +10730,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>551</v>
       </c>
@@ -10753,7 +10756,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>552</v>
       </c>
@@ -10779,7 +10782,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>553</v>
       </c>
@@ -10805,7 +10808,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>554</v>
       </c>
@@ -10831,7 +10834,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>555</v>
       </c>
@@ -10857,7 +10860,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>556</v>
       </c>
@@ -10883,7 +10886,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>557</v>
       </c>
@@ -10909,7 +10912,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>558</v>
       </c>
@@ -10935,7 +10938,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>559</v>
       </c>
@@ -10962,7 +10965,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H69"/>
+  <autoFilter ref="B2:H69">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SpW A"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -10970,9 +10979,12 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="B2:D268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10992,7 +11004,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>560</v>
       </c>
@@ -11004,7 +11016,7 @@
         <v>PIN_V12</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>560</v>
       </c>
@@ -11016,7 +11028,7 @@
         <v>2.5 V</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>561</v>
       </c>
@@ -11028,7 +11040,7 @@
         <v>PIN_V11</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>561</v>
       </c>
@@ -11040,7 +11052,7 @@
         <v>2.5 V</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>564</v>
       </c>
@@ -11052,7 +11064,7 @@
         <v>PIN_W7</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>564</v>
       </c>
@@ -11204,7 +11216,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>505</v>
       </c>
@@ -11216,7 +11228,7 @@
         <v>PIN_C9</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>505</v>
       </c>
@@ -11228,7 +11240,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>505</v>
       </c>
@@ -11239,7 +11251,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>504</v>
       </c>
@@ -11251,7 +11263,7 @@
         <v>PIN_D9</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>504</v>
       </c>
@@ -11263,7 +11275,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>504</v>
       </c>
@@ -11274,7 +11286,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>507</v>
       </c>
@@ -11286,7 +11298,7 @@
         <v>PIN_C8</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>507</v>
       </c>
@@ -11298,7 +11310,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>507</v>
       </c>
@@ -11309,7 +11321,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>506</v>
       </c>
@@ -11321,7 +11333,7 @@
         <v>PIN_D8</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>506</v>
       </c>
@@ -11333,7 +11345,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>506</v>
       </c>
@@ -11344,7 +11356,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>513</v>
       </c>
@@ -11356,7 +11368,7 @@
         <v>PIN_C7</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>513</v>
       </c>
@@ -11368,7 +11380,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>513</v>
       </c>
@@ -11379,7 +11391,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>512</v>
       </c>
@@ -11391,7 +11403,7 @@
         <v>PIN_D7</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>512</v>
       </c>
@@ -11403,7 +11415,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>512</v>
       </c>
@@ -11414,7 +11426,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>515</v>
       </c>
@@ -11426,7 +11438,7 @@
         <v>PIN_E10</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>515</v>
       </c>
@@ -11438,7 +11450,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>515</v>
       </c>
@@ -11449,7 +11461,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>514</v>
       </c>
@@ -11461,7 +11473,7 @@
         <v>PIN_F10</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>514</v>
       </c>
@@ -11473,7 +11485,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>514</v>
       </c>
@@ -11484,7 +11496,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>521</v>
       </c>
@@ -11496,7 +11508,7 @@
         <v>PIN_F5</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>521</v>
       </c>
@@ -11508,7 +11520,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>521</v>
       </c>
@@ -11519,7 +11531,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>520</v>
       </c>
@@ -11531,7 +11543,7 @@
         <v>PIN_G5</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>520</v>
       </c>
@@ -11543,7 +11555,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>520</v>
       </c>
@@ -11554,7 +11566,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>523</v>
       </c>
@@ -11566,7 +11578,7 @@
         <v>PIN_F6</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>523</v>
       </c>
@@ -11578,7 +11590,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>523</v>
       </c>
@@ -11589,7 +11601,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>522</v>
       </c>
@@ -11601,7 +11613,7 @@
         <v>PIN_G6</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>522</v>
       </c>
@@ -11613,7 +11625,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>522</v>
       </c>
@@ -11624,7 +11636,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>529</v>
       </c>
@@ -11636,7 +11648,7 @@
         <v>PIN_E7</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>529</v>
       </c>
@@ -11648,7 +11660,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>529</v>
       </c>
@@ -11659,7 +11671,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>528</v>
       </c>
@@ -11671,7 +11683,7 @@
         <v>PIN_F7</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>528</v>
       </c>
@@ -11683,7 +11695,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>528</v>
       </c>
@@ -11694,7 +11706,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>531</v>
       </c>
@@ -11706,7 +11718,7 @@
         <v>PIN_F8</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>531</v>
       </c>
@@ -11718,7 +11730,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>531</v>
       </c>
@@ -11729,7 +11741,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>530</v>
       </c>
@@ -11741,7 +11753,7 @@
         <v>PIN_G8</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>530</v>
       </c>
@@ -11753,7 +11765,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>530</v>
       </c>
@@ -11764,7 +11776,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>537</v>
       </c>
@@ -11776,7 +11788,7 @@
         <v>PIN_F9</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>537</v>
       </c>
@@ -11788,7 +11800,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>537</v>
       </c>
@@ -11799,7 +11811,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>536</v>
       </c>
@@ -11811,7 +11823,7 @@
         <v>PIN_G9</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>536</v>
       </c>
@@ -11823,7 +11835,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>536</v>
       </c>
@@ -11834,7 +11846,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
         <v>539</v>
       </c>
@@ -11846,7 +11858,7 @@
         <v>PIN_N5</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>539</v>
       </c>
@@ -11858,7 +11870,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>539</v>
       </c>
@@ -11869,7 +11881,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>538</v>
       </c>
@@ -11881,7 +11893,7 @@
         <v>PIN_N6</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>538</v>
       </c>
@@ -11893,7 +11905,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>538</v>
       </c>
@@ -11904,7 +11916,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>545</v>
       </c>
@@ -11916,7 +11928,7 @@
         <v>PIN_L5</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>545</v>
       </c>
@@ -11928,7 +11940,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>545</v>
       </c>
@@ -11939,7 +11951,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>544</v>
       </c>
@@ -11951,7 +11963,7 @@
         <v>PIN_M6</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>544</v>
       </c>
@@ -11963,7 +11975,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>544</v>
       </c>
@@ -11974,7 +11986,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>547</v>
       </c>
@@ -11986,7 +11998,7 @@
         <v>PIN_R5</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>547</v>
       </c>
@@ -11998,7 +12010,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>547</v>
       </c>
@@ -12009,7 +12021,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>546</v>
       </c>
@@ -12021,7 +12033,7 @@
         <v>PIN_R6</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>546</v>
       </c>
@@ -12033,7 +12045,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>546</v>
       </c>
@@ -12044,7 +12056,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>553</v>
       </c>
@@ -12056,7 +12068,7 @@
         <v>PIN_P6</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>553</v>
       </c>
@@ -12068,7 +12080,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>553</v>
       </c>
@@ -12079,7 +12091,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>552</v>
       </c>
@@ -12091,7 +12103,7 @@
         <v>PIN_R7</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>552</v>
       </c>
@@ -12103,7 +12115,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>552</v>
       </c>
@@ -12114,7 +12126,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
         <v>555</v>
       </c>
@@ -12126,7 +12138,7 @@
         <v>PIN_U5</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
         <v>555</v>
       </c>
@@ -12138,7 +12150,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
         <v>555</v>
       </c>
@@ -12149,7 +12161,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
         <v>554</v>
       </c>
@@ -12161,7 +12173,7 @@
         <v>PIN_V6</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
         <v>554</v>
       </c>
@@ -12173,7 +12185,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
         <v>554</v>
       </c>
@@ -12324,7 +12336,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>509</v>
       </c>
@@ -12336,7 +12348,7 @@
         <v>PIN_J9</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
         <v>509</v>
       </c>
@@ -12348,7 +12360,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
         <v>509</v>
       </c>
@@ -12359,7 +12371,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
         <v>508</v>
       </c>
@@ -12371,7 +12383,7 @@
         <v>PIN_K9</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
         <v>508</v>
       </c>
@@ -12383,7 +12395,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
         <v>508</v>
       </c>
@@ -12394,7 +12406,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
         <v>511</v>
       </c>
@@ -12406,7 +12418,7 @@
         <v>PIN_J10</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>511</v>
       </c>
@@ -12418,7 +12430,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
         <v>511</v>
       </c>
@@ -12429,7 +12441,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
         <v>510</v>
       </c>
@@ -12441,7 +12453,7 @@
         <v>PIN_K10</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
         <v>510</v>
       </c>
@@ -12453,7 +12465,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
         <v>510</v>
       </c>
@@ -12464,7 +12476,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
         <v>517</v>
       </c>
@@ -12476,7 +12488,7 @@
         <v>PIN_P13</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
         <v>517</v>
       </c>
@@ -12488,7 +12500,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
         <v>517</v>
       </c>
@@ -12499,7 +12511,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
         <v>516</v>
       </c>
@@ -12511,7 +12523,7 @@
         <v>PIN_R13</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
         <v>516</v>
       </c>
@@ -12523,7 +12535,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
         <v>516</v>
       </c>
@@ -12534,7 +12546,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
         <v>519</v>
       </c>
@@ -12546,7 +12558,7 @@
         <v>PIN_G7</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
         <v>519</v>
       </c>
@@ -12558,7 +12570,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B137" s="2" t="s">
         <v>519</v>
       </c>
@@ -12569,7 +12581,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B138" s="2" t="s">
         <v>518</v>
       </c>
@@ -12581,7 +12593,7 @@
         <v>PIN_H7</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B139" s="2" t="s">
         <v>518</v>
       </c>
@@ -12593,7 +12605,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
         <v>518</v>
       </c>
@@ -12604,7 +12616,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B141" s="2" t="s">
         <v>525</v>
       </c>
@@ -12616,7 +12628,7 @@
         <v>PIN_R11</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
         <v>525</v>
       </c>
@@ -12628,7 +12640,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B143" s="2" t="s">
         <v>525</v>
       </c>
@@ -12639,7 +12651,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
         <v>524</v>
       </c>
@@ -12651,7 +12663,7 @@
         <v>PIN_R12</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B145" s="2" t="s">
         <v>524</v>
       </c>
@@ -12663,7 +12675,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B146" s="2" t="s">
         <v>524</v>
       </c>
@@ -12674,7 +12686,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
         <v>527</v>
       </c>
@@ -12686,7 +12698,7 @@
         <v>PIN_T12</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B148" s="2" t="s">
         <v>527</v>
       </c>
@@ -12698,7 +12710,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B149" s="2" t="s">
         <v>527</v>
       </c>
@@ -12709,7 +12721,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B150" s="2" t="s">
         <v>526</v>
       </c>
@@ -12721,7 +12733,7 @@
         <v>PIN_T13</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B151" s="2" t="s">
         <v>526</v>
       </c>
@@ -12733,7 +12745,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="2" t="s">
         <v>526</v>
       </c>
@@ -12744,7 +12756,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B153" s="2" t="s">
         <v>533</v>
       </c>
@@ -12756,7 +12768,7 @@
         <v>PIN_L11</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B154" s="2" t="s">
         <v>533</v>
       </c>
@@ -12768,7 +12780,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B155" s="2" t="s">
         <v>533</v>
       </c>
@@ -12779,7 +12791,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
         <v>532</v>
       </c>
@@ -12791,7 +12803,7 @@
         <v>PIN_M11</v>
       </c>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
         <v>532</v>
       </c>
@@ -12803,7 +12815,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B158" s="2" t="s">
         <v>532</v>
       </c>
@@ -12814,7 +12826,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B159" s="2" t="s">
         <v>535</v>
       </c>
@@ -12826,7 +12838,7 @@
         <v>PIN_P8</v>
       </c>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
         <v>535</v>
       </c>
@@ -12838,7 +12850,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
         <v>535</v>
       </c>
@@ -12849,7 +12861,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
         <v>534</v>
       </c>
@@ -12861,7 +12873,7 @@
         <v>PIN_N9</v>
       </c>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
         <v>534</v>
       </c>
@@ -12873,7 +12885,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B164" s="2" t="s">
         <v>534</v>
       </c>
@@ -12884,7 +12896,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B165" s="2" t="s">
         <v>541</v>
       </c>
@@ -12896,7 +12908,7 @@
         <v>PIN_L10</v>
       </c>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B166" s="2" t="s">
         <v>541</v>
       </c>
@@ -12908,7 +12920,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B167" s="2" t="s">
         <v>541</v>
       </c>
@@ -12919,7 +12931,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B168" s="2" t="s">
         <v>540</v>
       </c>
@@ -12931,7 +12943,7 @@
         <v>PIN_M10</v>
       </c>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
         <v>540</v>
       </c>
@@ -12943,7 +12955,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B170" s="2" t="s">
         <v>540</v>
       </c>
@@ -12954,7 +12966,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B171" s="2" t="s">
         <v>543</v>
       </c>
@@ -12966,7 +12978,7 @@
         <v>PIN_M7</v>
       </c>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B172" s="2" t="s">
         <v>543</v>
       </c>
@@ -12978,7 +12990,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
         <v>543</v>
       </c>
@@ -12989,7 +13001,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B174" s="2" t="s">
         <v>542</v>
       </c>
@@ -13001,7 +13013,7 @@
         <v>PIN_M8</v>
       </c>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B175" s="2" t="s">
         <v>542</v>
       </c>
@@ -13013,7 +13025,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B176" s="2" t="s">
         <v>542</v>
       </c>
@@ -13024,7 +13036,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B177" s="2" t="s">
         <v>549</v>
       </c>
@@ -13036,7 +13048,7 @@
         <v>PIN_V9</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B178" s="2" t="s">
         <v>549</v>
       </c>
@@ -13048,7 +13060,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B179" s="2" t="s">
         <v>549</v>
       </c>
@@ -13059,7 +13071,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B180" s="2" t="s">
         <v>548</v>
       </c>
@@ -13071,7 +13083,7 @@
         <v>PIN_V10</v>
       </c>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
         <v>548</v>
       </c>
@@ -13083,7 +13095,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B182" s="2" t="s">
         <v>548</v>
       </c>
@@ -13094,7 +13106,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B183" s="2" t="s">
         <v>551</v>
       </c>
@@ -13106,7 +13118,7 @@
         <v>PIN_R10</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B184" s="2" t="s">
         <v>551</v>
       </c>
@@ -13118,7 +13130,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B185" s="2" t="s">
         <v>551</v>
       </c>
@@ -13129,7 +13141,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B186" s="2" t="s">
         <v>550</v>
       </c>
@@ -13141,7 +13153,7 @@
         <v>PIN_T10</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B187" s="2" t="s">
         <v>550</v>
       </c>
@@ -13153,7 +13165,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B188" s="2" t="s">
         <v>550</v>
       </c>
@@ -13164,7 +13176,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B189" s="2" t="s">
         <v>557</v>
       </c>
@@ -13176,7 +13188,7 @@
         <v>PIN_R8</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
         <v>557</v>
       </c>
@@ -13188,7 +13200,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B191" s="2" t="s">
         <v>557</v>
       </c>
@@ -13199,7 +13211,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B192" s="2" t="s">
         <v>556</v>
       </c>
@@ -13211,7 +13223,7 @@
         <v>PIN_R9</v>
       </c>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B193" s="2" t="s">
         <v>556</v>
       </c>
@@ -13223,7 +13235,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B194" s="2" t="s">
         <v>556</v>
       </c>
@@ -13234,7 +13246,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B195" s="2" t="s">
         <v>559</v>
       </c>
@@ -13246,7 +13258,7 @@
         <v>PIN_T9</v>
       </c>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B196" s="2" t="s">
         <v>559</v>
       </c>
@@ -13258,7 +13270,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B197" s="2" t="s">
         <v>559</v>
       </c>
@@ -13269,7 +13281,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B198" s="2" t="s">
         <v>558</v>
       </c>
@@ -13281,7 +13293,7 @@
         <v>PIN_U10</v>
       </c>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
         <v>558</v>
       </c>
@@ -13293,7 +13305,7 @@
         <v>LVDS</v>
       </c>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B200" s="2" t="s">
         <v>558</v>
       </c>
@@ -13507,6 +13519,18 @@
     </row>
   </sheetData>
   <autoFilter ref="B2:D200">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="HSMB_LVDS_RX_SPWA_DI_N"/>
+        <filter val="HSMB_LVDS_RX_SPWA_DI_P"/>
+        <filter val="HSMB_LVDS_RX_SPWA_SI_N"/>
+        <filter val="HSMB_LVDS_RX_SPWA_SI_P"/>
+        <filter val="HSMB_LVDS_TX_SPWA_DO_N"/>
+        <filter val="HSMB_LVDS_TX_SPWA_DO_P"/>
+        <filter val="HSMB_LVDS_TX_SPWA_SO_N"/>
+        <filter val="HSMB_LVDS_TX_SPWA_SO_P"/>
+      </filters>
+    </filterColumn>
     <sortState ref="B3:D200">
       <sortCondition ref="B2:B200"/>
     </sortState>

</xml_diff>